<commit_message>
changed kappa column from % to numeric
</commit_message>
<xml_diff>
--- a/Project dashboard.xlsx
+++ b/Project dashboard.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://leedsbeckett-my.sharepoint.com/personal/j_skelton3558_student_leedsbeckett_ac_uk/Documents/Year 3/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="469" documentId="8_{03931816-D41B-414A-B0D9-A11D16A90E45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39B20AB4-4F2A-4ECA-B3B2-AFFBDABD69F6}"/>
+  <xr:revisionPtr revIDLastSave="472" documentId="8_{03931816-D41B-414A-B0D9-A11D16A90E45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{740A777A-9391-43E9-A986-58247B747178}"/>
   <bookViews>
-    <workbookView xWindow="16080" yWindow="5625" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{280908C4-F3F2-4359-9CF5-347137099EA1}"/>
+    <workbookView xWindow="16080" yWindow="5625" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{280908C4-F3F2-4359-9CF5-347137099EA1}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
-    <sheet name="dashboard" sheetId="2" r:id="rId2"/>
+    <sheet name="Detail1" sheetId="3" r:id="rId2"/>
+    <sheet name="dashboard" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v2.0" hidden="1">data!$B$3:$B$7</definedName>
@@ -25,12 +26,12 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
       <x14:slicerCaches>
-        <x14:slicerCache r:id="rId4"/>
+        <x14:slicerCache r:id="rId5"/>
       </x14:slicerCaches>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
   <si>
     <t>model</t>
   </si>
@@ -110,12 +111,15 @@
   <si>
     <t>Models</t>
   </si>
+  <si>
+    <t>Details for Sum of kappa - model: decision tree</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +129,14 @@
     </font>
     <font>
       <sz val="28"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -169,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -185,11 +197,79 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="24">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFF9D6B9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFF9D6B9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFF9D6B9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFF9D6B9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFF9D6B9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -721,7 +801,7 @@
             <c:numRef>
               <c:f>dashboard!$H$12:$H$16</c:f>
               <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.35360000000000003</c:v>
@@ -2278,7 +2358,7 @@
             <c:numRef>
               <c:f>dashboard!$H$12:$H$16</c:f>
               <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.35360000000000003</c:v>
@@ -6700,16 +6780,16 @@
         <a:lstStyle/>
         <a:p>
           <a:fld id="{E64D1D14-AB1D-40A1-AF8B-A08592DE3F5D}" type="TxLink">
-            <a:rPr lang="en-US" sz="2800" b="0" i="0" u="none" strike="noStrike">
+            <a:rPr lang="en-US" sz="3600" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
               <a:latin typeface="Aptos Narrow"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>35.36%</a:t>
+            <a:t>0.35</a:t>
           </a:fld>
-          <a:endParaRPr lang="en-GB" sz="6000"/>
+          <a:endParaRPr lang="en-GB" sz="7200"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -7318,29 +7398,29 @@
   </colItems>
   <dataFields count="5">
     <dataField name="Sum of accuracy" fld="1" baseField="0" baseItem="0" numFmtId="10"/>
-    <dataField name="Sum of kappa" fld="2" baseField="0" baseItem="0" numFmtId="10"/>
+    <dataField name="Sum of kappa" fld="2" baseField="0" baseItem="0" numFmtId="2"/>
     <dataField name="Sum of sensitivity" fld="3" baseField="0" baseItem="0" numFmtId="10"/>
     <dataField name="Sum of specificity" fld="4" baseField="0" baseItem="0" numFmtId="10"/>
     <dataField name="Sum of detection rate" fld="5" baseField="0" baseItem="0" numFmtId="10"/>
   </dataFields>
-  <formats count="9">
-    <format dxfId="8">
+  <formats count="10">
+    <format dxfId="18">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="7">
+    <format dxfId="17">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="6">
+    <format dxfId="16">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="5">
+    <format dxfId="15">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="4">
+    <format dxfId="14">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="5">
@@ -7353,10 +7433,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="13">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="2">
+    <format dxfId="12">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="5">
@@ -7369,24 +7449,55 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="11">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="0">
+    <format dxfId="10">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
+    <format dxfId="0">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
   </formats>
   <conditionalFormats count="5">
-    <conditionalFormat priority="5">
+    <conditionalFormat priority="1">
       <pivotAreas count="1">
         <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="1">
             <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
+              <x v="4"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="2">
+      <pivotAreas count="1">
+        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="3"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="3">
+      <pivotAreas count="1">
+        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="2"/>
             </reference>
           </references>
         </pivotArea>
@@ -7403,34 +7514,12 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat priority="3">
+    <conditionalFormat priority="5">
       <pivotAreas count="1">
         <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="1">
             <reference field="4294967294" count="1" selected="0">
-              <x v="2"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="2">
-      <pivotAreas count="1">
-        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="3"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="1">
-      <pivotAreas count="1">
-        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="4"/>
+              <x v="0"/>
             </reference>
           </references>
         </pivotArea>
@@ -7871,13 +7960,31 @@
   <autoFilter ref="B2:G7" xr:uid="{EF765BF0-0E6E-4F06-A7EC-50E59049A84F}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{9CA3639C-9338-4E6C-9D14-99F464F3B40B}" name="model"/>
-    <tableColumn id="2" xr3:uid="{0134932A-9966-484A-951F-71881E4B1DE3}" name="accuracy" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{0048ACCC-8730-48B1-8DE1-17D7B2382E71}" name="kappa" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{B819A17C-D9D5-46C6-8805-6EBB6FA1BAFF}" name="sensitivity" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{699561B5-91DE-448A-8631-061EACA78401}" name="specificity" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{74C63BD7-ADCD-4520-8DAF-DBF8153580C4}" name="detection rate" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{0134932A-9966-484A-951F-71881E4B1DE3}" name="accuracy" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{0048ACCC-8730-48B1-8DE1-17D7B2382E71}" name="kappa" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{B819A17C-D9D5-46C6-8805-6EBB6FA1BAFF}" name="sensitivity" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{699561B5-91DE-448A-8631-061EACA78401}" name="specificity" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{74C63BD7-ADCD-4520-8DAF-DBF8153580C4}" name="detection rate" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9B467EC7-E6CE-43B4-AAAC-6153E6E2CA29}" name="Table2" displayName="Table2" ref="A3:F4" totalsRowShown="0">
+  <autoFilter ref="A3:F4" xr:uid="{9B467EC7-E6CE-43B4-AAAC-6153E6E2CA29}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:F4">
+    <sortCondition ref="C3:C4"/>
+  </sortState>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{3A40107B-F282-4229-A676-F10EEBD4A784}" name="model"/>
+    <tableColumn id="2" xr3:uid="{7594E9E6-ABA3-46C0-89DF-A4F6249BEA5B}" name="accuracy"/>
+    <tableColumn id="3" xr3:uid="{8DE7357B-246E-44E3-B39F-9447BCE633A7}" name="kappa"/>
+    <tableColumn id="4" xr3:uid="{029E6700-FE04-42C9-829F-7211DA2F72D6}" name="sensitivity"/>
+    <tableColumn id="5" xr3:uid="{338C7D83-E796-4BFE-85CD-530F3C4DCA69}" name="specificity"/>
+    <tableColumn id="6" xr3:uid="{E766E66E-C38A-44B5-A59B-51FB1FE96D78}" name="detection rate"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -8447,11 +8554,81 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADB379C9-8D42-461A-B331-BA92C6036B5A}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>0.82069999999999999</v>
+      </c>
+      <c r="C4">
+        <v>0.35360000000000003</v>
+      </c>
+      <c r="D4">
+        <v>0.95879999999999999</v>
+      </c>
+      <c r="E4">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="F4">
+        <v>0.89600000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2087B8DC-4C91-4FD0-A29B-B3D8CACCA267}">
   <dimension ref="A1:AH59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12:K16"/>
+      <selection activeCell="AE14" sqref="AE14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8886,7 +9063,7 @@
       <c r="G12" s="7">
         <v>0.82069999999999999</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="10">
         <v>0.35360000000000003</v>
       </c>
       <c r="I12" s="7">
@@ -8934,7 +9111,7 @@
       <c r="G13" s="7">
         <v>0.79349999999999998</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="10">
         <v>0.31080000000000002</v>
       </c>
       <c r="I13" s="7">
@@ -8982,7 +9159,7 @@
       <c r="G14" s="7">
         <v>0.81120000000000003</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H14" s="10">
         <v>0.29930000000000001</v>
       </c>
       <c r="I14" s="7">
@@ -9030,7 +9207,7 @@
       <c r="G15" s="7">
         <v>0.69410000000000005</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="10">
         <v>0.30009999999999998</v>
       </c>
       <c r="I15" s="7">
@@ -9078,7 +9255,7 @@
       <c r="G16" s="7">
         <v>0.81720000000000004</v>
       </c>
-      <c r="H16" s="7">
+      <c r="H16" s="10">
         <v>0.37359999999999999</v>
       </c>
       <c r="I16" s="7">
@@ -10740,6 +10917,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="62b2270f-cac5-4cb0-a3fe-00132c744b99" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001E04701497BB6E42B560D138C93E4319" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0fa9e4b1cf3f9216a8992511e21091a7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="62b2270f-cac5-4cb0-a3fe-00132c744b99" xmlns:ns4="579371f9-af73-4890-8fa4-4b906fbd19c2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c2c0f297db49476ddbe35a586431e862" ns3:_="" ns4:_="">
     <xsd:import namespace="62b2270f-cac5-4cb0-a3fe-00132c744b99"/>
@@ -10966,24 +11160,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0691411-F348-464D-ADBE-45D548823D8E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="62b2270f-cac5-4cb0-a3fe-00132c744b99"/>
+    <ds:schemaRef ds:uri="579371f9-af73-4890-8fa4-4b906fbd19c2"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="62b2270f-cac5-4cb0-a3fe-00132c744b99" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8246D7A6-CBAB-45FC-957A-05D07DEF6357}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BFA038C-F644-489C-9938-D66D1680E46B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11000,29 +11202,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8246D7A6-CBAB-45FC-957A-05D07DEF6357}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0691411-F348-464D-ADBE-45D548823D8E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="62b2270f-cac5-4cb0-a3fe-00132c744b99"/>
-    <ds:schemaRef ds:uri="579371f9-af73-4890-8fa4-4b906fbd19c2"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>